<commit_message>
Debug on small trajectory
</commit_message>
<xml_diff>
--- a/experiments/pg/return_discount_increment/max_rew_mlp_3x256_corr_entropy_inp_time_step_3e_4_no_norm/oracle_buffer.xlsx
+++ b/experiments/pg/return_discount_increment/max_rew_mlp_3x256_corr_entropy_inp_time_step_3e_4_no_norm/oracle_buffer.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2514"/>
+  <dimension ref="A1:C2562"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -33114,6 +33114,630 @@
         <v>15.16302322931569</v>
       </c>
     </row>
+    <row r="2515">
+      <c r="A2515" s="1" t="n">
+        <v>2513</v>
+      </c>
+      <c r="B2515" t="inlineStr">
+        <is>
+          <t>[0, -7, 5]</t>
+        </is>
+      </c>
+      <c r="C2515" t="n">
+        <v>15.28572233692817</v>
+      </c>
+    </row>
+    <row r="2516">
+      <c r="A2516" s="1" t="n">
+        <v>2514</v>
+      </c>
+      <c r="B2516" t="inlineStr">
+        <is>
+          <t>[4, -1, 7]</t>
+        </is>
+      </c>
+      <c r="C2516" t="n">
+        <v>14.23819195963161</v>
+      </c>
+    </row>
+    <row r="2517">
+      <c r="A2517" s="1" t="n">
+        <v>2515</v>
+      </c>
+      <c r="B2517" t="inlineStr">
+        <is>
+          <t>[3, -2, 6]</t>
+        </is>
+      </c>
+      <c r="C2517" t="n">
+        <v>14.49239652783319</v>
+      </c>
+    </row>
+    <row r="2518">
+      <c r="A2518" s="1" t="n">
+        <v>2516</v>
+      </c>
+      <c r="B2518" t="inlineStr">
+        <is>
+          <t>[5, 0, 7]</t>
+        </is>
+      </c>
+      <c r="C2518" t="n">
+        <v>14.2916524203619</v>
+      </c>
+    </row>
+    <row r="2519">
+      <c r="A2519" s="1" t="n">
+        <v>2517</v>
+      </c>
+      <c r="B2519" t="inlineStr">
+        <is>
+          <t>[2, -2, 6]</t>
+        </is>
+      </c>
+      <c r="C2519" t="n">
+        <v>15.46022536371772</v>
+      </c>
+    </row>
+    <row r="2520">
+      <c r="A2520" s="1" t="n">
+        <v>2518</v>
+      </c>
+      <c r="B2520" t="inlineStr">
+        <is>
+          <t>[5, 0, 6]</t>
+        </is>
+      </c>
+      <c r="C2520" t="n">
+        <v>14.38537152011593</v>
+      </c>
+    </row>
+    <row r="2521">
+      <c r="A2521" s="1" t="n">
+        <v>2519</v>
+      </c>
+      <c r="B2521" t="inlineStr">
+        <is>
+          <t>[3, -3, 6]</t>
+        </is>
+      </c>
+      <c r="C2521" t="n">
+        <v>14.23435105656958</v>
+      </c>
+    </row>
+    <row r="2522">
+      <c r="A2522" s="1" t="n">
+        <v>2520</v>
+      </c>
+      <c r="B2522" t="inlineStr">
+        <is>
+          <t>[3, -3, 5]</t>
+        </is>
+      </c>
+      <c r="C2522" t="n">
+        <v>14.33962475017112</v>
+      </c>
+    </row>
+    <row r="2523">
+      <c r="A2523" s="1" t="n">
+        <v>2521</v>
+      </c>
+      <c r="B2523" t="inlineStr">
+        <is>
+          <t>[3, -2, 7]</t>
+        </is>
+      </c>
+      <c r="C2523" t="n">
+        <v>14.43950852768009</v>
+      </c>
+    </row>
+    <row r="2524">
+      <c r="A2524" s="1" t="n">
+        <v>2522</v>
+      </c>
+      <c r="B2524" t="inlineStr">
+        <is>
+          <t>[2, -3, 6]</t>
+        </is>
+      </c>
+      <c r="C2524" t="n">
+        <v>14.68058402331847</v>
+      </c>
+    </row>
+    <row r="2525">
+      <c r="A2525" s="1" t="n">
+        <v>2523</v>
+      </c>
+      <c r="B2525" t="inlineStr">
+        <is>
+          <t>[2, -4, 6]</t>
+        </is>
+      </c>
+      <c r="C2525" t="n">
+        <v>14.67877272011704</v>
+      </c>
+    </row>
+    <row r="2526">
+      <c r="A2526" s="1" t="n">
+        <v>2524</v>
+      </c>
+      <c r="B2526" t="inlineStr">
+        <is>
+          <t>[5, -7, -2]</t>
+        </is>
+      </c>
+      <c r="C2526" t="n">
+        <v>13.98585790195392</v>
+      </c>
+    </row>
+    <row r="2527">
+      <c r="A2527" s="1" t="n">
+        <v>2525</v>
+      </c>
+      <c r="B2527" t="inlineStr">
+        <is>
+          <t>[4, -2, 7]</t>
+        </is>
+      </c>
+      <c r="C2527" t="n">
+        <v>14.0374308942397</v>
+      </c>
+    </row>
+    <row r="2528">
+      <c r="A2528" s="1" t="n">
+        <v>2526</v>
+      </c>
+      <c r="B2528" t="inlineStr">
+        <is>
+          <t>[5, -1, 7]</t>
+        </is>
+      </c>
+      <c r="C2528" t="n">
+        <v>14.20636515333507</v>
+      </c>
+    </row>
+    <row r="2529">
+      <c r="A2529" s="1" t="n">
+        <v>2527</v>
+      </c>
+      <c r="B2529" t="inlineStr">
+        <is>
+          <t>[2, -2, 7]</t>
+        </is>
+      </c>
+      <c r="C2529" t="n">
+        <v>15.47987207469113</v>
+      </c>
+    </row>
+    <row r="2530">
+      <c r="A2530" s="1" t="n">
+        <v>2528</v>
+      </c>
+      <c r="B2530" t="inlineStr">
+        <is>
+          <t>[3, -4, 5]</t>
+        </is>
+      </c>
+      <c r="C2530" t="n">
+        <v>14.34796612566152</v>
+      </c>
+    </row>
+    <row r="2531">
+      <c r="A2531" s="1" t="n">
+        <v>2529</v>
+      </c>
+      <c r="B2531" t="inlineStr">
+        <is>
+          <t>[3, -3, 7]</t>
+        </is>
+      </c>
+      <c r="C2531" t="n">
+        <v>14.21189433694705</v>
+      </c>
+    </row>
+    <row r="2532">
+      <c r="A2532" s="1" t="n">
+        <v>2530</v>
+      </c>
+      <c r="B2532" t="inlineStr">
+        <is>
+          <t>[4, -2, 6]</t>
+        </is>
+      </c>
+      <c r="C2532" t="n">
+        <v>14.09966332257641</v>
+      </c>
+    </row>
+    <row r="2533">
+      <c r="A2533" s="1" t="n">
+        <v>2531</v>
+      </c>
+      <c r="B2533" t="inlineStr">
+        <is>
+          <t>[4, -2, 5]</t>
+        </is>
+      </c>
+      <c r="C2533" t="n">
+        <v>14.15908284861707</v>
+      </c>
+    </row>
+    <row r="2534">
+      <c r="A2534" s="1" t="n">
+        <v>2532</v>
+      </c>
+      <c r="B2534" t="inlineStr">
+        <is>
+          <t>[4, -3, 5]</t>
+        </is>
+      </c>
+      <c r="C2534" t="n">
+        <v>14.06777833042299</v>
+      </c>
+    </row>
+    <row r="2535">
+      <c r="A2535" s="1" t="n">
+        <v>2533</v>
+      </c>
+      <c r="B2535" t="inlineStr">
+        <is>
+          <t>[3, -4, 6]</t>
+        </is>
+      </c>
+      <c r="C2535" t="n">
+        <v>14.24142405702893</v>
+      </c>
+    </row>
+    <row r="2536">
+      <c r="A2536" s="1" t="n">
+        <v>2534</v>
+      </c>
+      <c r="B2536" t="inlineStr">
+        <is>
+          <t>[6, 0, 7]</t>
+        </is>
+      </c>
+      <c r="C2536" t="n">
+        <v>14.68923399284561</v>
+      </c>
+    </row>
+    <row r="2537">
+      <c r="A2537" s="1" t="n">
+        <v>2535</v>
+      </c>
+      <c r="B2537" t="inlineStr">
+        <is>
+          <t>[6, -1, 6]</t>
+        </is>
+      </c>
+      <c r="C2537" t="n">
+        <v>14.3511995564321</v>
+      </c>
+    </row>
+    <row r="2538">
+      <c r="A2538" s="1" t="n">
+        <v>2536</v>
+      </c>
+      <c r="B2538" t="inlineStr">
+        <is>
+          <t>[5, -2, 5]</t>
+        </is>
+      </c>
+      <c r="C2538" t="n">
+        <v>13.98439257477286</v>
+      </c>
+    </row>
+    <row r="2539">
+      <c r="A2539" s="1" t="n">
+        <v>2537</v>
+      </c>
+      <c r="B2539" t="inlineStr">
+        <is>
+          <t>[6, -1, 7]</t>
+        </is>
+      </c>
+      <c r="C2539" t="n">
+        <v>14.37562758966072</v>
+      </c>
+    </row>
+    <row r="2540">
+      <c r="A2540" s="1" t="n">
+        <v>2538</v>
+      </c>
+      <c r="B2540" t="inlineStr">
+        <is>
+          <t>[6, -6, -1]</t>
+        </is>
+      </c>
+      <c r="C2540" t="n">
+        <v>14.35937706818516</v>
+      </c>
+    </row>
+    <row r="2541">
+      <c r="A2541" s="1" t="n">
+        <v>2539</v>
+      </c>
+      <c r="B2541" t="inlineStr">
+        <is>
+          <t>[6, -7, -2]</t>
+        </is>
+      </c>
+      <c r="C2541" t="n">
+        <v>14.0678058912073</v>
+      </c>
+    </row>
+    <row r="2542">
+      <c r="A2542" s="1" t="n">
+        <v>2540</v>
+      </c>
+      <c r="B2542" t="inlineStr">
+        <is>
+          <t>[5, -2, 4]</t>
+        </is>
+      </c>
+      <c r="C2542" t="n">
+        <v>14.15424887767322</v>
+      </c>
+    </row>
+    <row r="2543">
+      <c r="A2543" s="1" t="n">
+        <v>2541</v>
+      </c>
+      <c r="B2543" t="inlineStr">
+        <is>
+          <t>[7, -5, -2]</t>
+        </is>
+      </c>
+      <c r="C2543" t="n">
+        <v>14.08510830348672</v>
+      </c>
+    </row>
+    <row r="2544">
+      <c r="A2544" s="1" t="n">
+        <v>2542</v>
+      </c>
+      <c r="B2544" t="inlineStr">
+        <is>
+          <t>[3, 7, -2]</t>
+        </is>
+      </c>
+      <c r="C2544" t="n">
+        <v>14.43950852800636</v>
+      </c>
+    </row>
+    <row r="2545">
+      <c r="A2545" s="1" t="n">
+        <v>2543</v>
+      </c>
+      <c r="B2545" t="inlineStr">
+        <is>
+          <t>[4, -7, -3]</t>
+        </is>
+      </c>
+      <c r="C2545" t="n">
+        <v>13.98245047374972</v>
+      </c>
+    </row>
+    <row r="2546">
+      <c r="A2546" s="1" t="n">
+        <v>2544</v>
+      </c>
+      <c r="B2546" t="inlineStr">
+        <is>
+          <t>[6, -6, -3]</t>
+        </is>
+      </c>
+      <c r="C2546" t="n">
+        <v>14.01078430776325</v>
+      </c>
+    </row>
+    <row r="2547">
+      <c r="A2547" s="1" t="n">
+        <v>2545</v>
+      </c>
+      <c r="B2547" t="inlineStr">
+        <is>
+          <t>[7, -6, -3]</t>
+        </is>
+      </c>
+      <c r="C2547" t="n">
+        <v>14.00527186733722</v>
+      </c>
+    </row>
+    <row r="2548">
+      <c r="A2548" s="1" t="n">
+        <v>2546</v>
+      </c>
+      <c r="B2548" t="inlineStr">
+        <is>
+          <t>[7, -1, 6]</t>
+        </is>
+      </c>
+      <c r="C2548" t="n">
+        <v>14.36654541156535</v>
+      </c>
+    </row>
+    <row r="2549">
+      <c r="A2549" s="1" t="n">
+        <v>2547</v>
+      </c>
+      <c r="B2549" t="inlineStr">
+        <is>
+          <t>[7, 1, 3]</t>
+        </is>
+      </c>
+      <c r="C2549" t="n">
+        <v>14.97396957082438</v>
+      </c>
+    </row>
+    <row r="2550">
+      <c r="A2550" s="1" t="n">
+        <v>2548</v>
+      </c>
+      <c r="B2550" t="inlineStr">
+        <is>
+          <t>[6, -2, 3]</t>
+        </is>
+      </c>
+      <c r="C2550" t="n">
+        <v>14.15615621406356</v>
+      </c>
+    </row>
+    <row r="2551">
+      <c r="A2551" s="1" t="n">
+        <v>2549</v>
+      </c>
+      <c r="B2551" t="inlineStr">
+        <is>
+          <t>[7, 1, 2]</t>
+        </is>
+      </c>
+      <c r="C2551" t="n">
+        <v>14.93359506072333</v>
+      </c>
+    </row>
+    <row r="2552">
+      <c r="A2552" s="1" t="n">
+        <v>2550</v>
+      </c>
+      <c r="B2552" t="inlineStr">
+        <is>
+          <t>[1, 7, -2]</t>
+        </is>
+      </c>
+      <c r="C2552" t="n">
+        <v>16.20788697882952</v>
+      </c>
+    </row>
+    <row r="2553">
+      <c r="A2553" s="1" t="n">
+        <v>2551</v>
+      </c>
+      <c r="B2553" t="inlineStr">
+        <is>
+          <t>[1, -3, 6]</t>
+        </is>
+      </c>
+      <c r="C2553" t="n">
+        <v>15.19884109298317</v>
+      </c>
+    </row>
+    <row r="2554">
+      <c r="A2554" s="1" t="n">
+        <v>2552</v>
+      </c>
+      <c r="B2554" t="inlineStr">
+        <is>
+          <t>[1, -3, 7]</t>
+        </is>
+      </c>
+      <c r="C2554" t="n">
+        <v>15.21355883566591</v>
+      </c>
+    </row>
+    <row r="2555">
+      <c r="A2555" s="1" t="n">
+        <v>2553</v>
+      </c>
+      <c r="B2555" t="inlineStr">
+        <is>
+          <t>[2, -3, 7]</t>
+        </is>
+      </c>
+      <c r="C2555" t="n">
+        <v>14.69790549308267</v>
+      </c>
+    </row>
+    <row r="2556">
+      <c r="A2556" s="1" t="n">
+        <v>2554</v>
+      </c>
+      <c r="B2556" t="inlineStr">
+        <is>
+          <t>[0, -3, 7]</t>
+        </is>
+      </c>
+      <c r="C2556" t="n">
+        <v>15.33528636979073</v>
+      </c>
+    </row>
+    <row r="2557">
+      <c r="A2557" s="1" t="n">
+        <v>2555</v>
+      </c>
+      <c r="B2557" t="inlineStr">
+        <is>
+          <t>[2, -4, 7]</t>
+        </is>
+      </c>
+      <c r="C2557" t="n">
+        <v>14.69712175326478</v>
+      </c>
+    </row>
+    <row r="2558">
+      <c r="A2558" s="1" t="n">
+        <v>2556</v>
+      </c>
+      <c r="B2558" t="inlineStr">
+        <is>
+          <t>[1, -4, 7]</t>
+        </is>
+      </c>
+      <c r="C2558" t="n">
+        <v>15.1770709824043</v>
+      </c>
+    </row>
+    <row r="2559">
+      <c r="A2559" s="1" t="n">
+        <v>2557</v>
+      </c>
+      <c r="B2559" t="inlineStr">
+        <is>
+          <t>[1, -5, 7]</t>
+        </is>
+      </c>
+      <c r="C2559" t="n">
+        <v>15.17628761134422</v>
+      </c>
+    </row>
+    <row r="2560">
+      <c r="A2560" s="1" t="n">
+        <v>2558</v>
+      </c>
+      <c r="B2560" t="inlineStr">
+        <is>
+          <t>[1, -6, 7]</t>
+        </is>
+      </c>
+      <c r="C2560" t="n">
+        <v>15.17868816231102</v>
+      </c>
+    </row>
+    <row r="2561">
+      <c r="A2561" s="1" t="n">
+        <v>2559</v>
+      </c>
+      <c r="B2561" t="inlineStr">
+        <is>
+          <t>[1, -6, 6]</t>
+        </is>
+      </c>
+      <c r="C2561" t="n">
+        <v>15.16379453357068</v>
+      </c>
+    </row>
+    <row r="2562">
+      <c r="A2562" s="1" t="n">
+        <v>2560</v>
+      </c>
+      <c r="B2562" t="inlineStr">
+        <is>
+          <t>[2, -5, 7]</t>
+        </is>
+      </c>
+      <c r="C2562" t="n">
+        <v>14.69425127571442</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>